<commit_message>
Update LSA Data Dictionary FY2023.xlsx
addresses #1111
</commit_message>
<xml_diff>
--- a/LSA Data Dictionary FY2023.xlsx
+++ b/LSA Data Dictionary FY2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://squarepegdata-my.sharepoint.com/personal/molly_squarepegdata_com/Documents/GitHub/LSASampleCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{84A0A88E-B7F7-4E6A-BAE7-02FF3B7B69D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5EB45F3-41AD-4DCC-BC55-23ACE5F3FEC5}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{84A0A88E-B7F7-4E6A-BAE7-02FF3B7B69D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7415522-0B2F-4004-BEAB-11B562CF8C5B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-27645" yWindow="-90" windowWidth="13830" windowHeight="6045" activeTab="2" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Columns!$A$1:$J$289</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Lists!$A$1:$XFB$1090</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Lists!$A$1:$XFB$1093</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="1563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3896" uniqueCount="1566">
   <si>
     <t>File ID</t>
   </si>
@@ -4746,6 +4746,15 @@
   </si>
   <si>
     <t>Domestic Violence Survivors Not Identified as Currently Fleeing</t>
+  </si>
+  <si>
+    <t>Veteran - Domestic Violence Survivor Not Identified as Currently Fleeing</t>
+  </si>
+  <si>
+    <t>Parenting Youth 18-24 - Domestic Violence Survivor Not Identified as Currently Fleeing</t>
+  </si>
+  <si>
+    <t>Parenting Child - Domestic Violence Survivor Not Identified as Currently Fleeing</t>
   </si>
 </sst>
 </file>
@@ -4979,6 +4988,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13520,11 +13533,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B52880F-20AD-49BC-9FD8-A02C6FD116A7}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N1090"/>
+  <dimension ref="A1:N1093"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G551" sqref="G551"/>
+      <pane ySplit="1" topLeftCell="A867" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D892" sqref="D892"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -24895,11 +24908,11 @@
       <c r="B805" t="s">
         <v>313</v>
       </c>
-      <c r="C805" s="13">
-        <v>5153</v>
-      </c>
-      <c r="D805" t="s">
-        <v>1384</v>
+      <c r="C805" s="34">
+        <v>5097</v>
+      </c>
+      <c r="D805" s="29" t="s">
+        <v>1563</v>
       </c>
     </row>
     <row r="806" spans="1:4" x14ac:dyDescent="0.45">
@@ -24910,10 +24923,10 @@
         <v>313</v>
       </c>
       <c r="C806" s="13">
-        <v>5154</v>
+        <v>5153</v>
       </c>
       <c r="D806" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="807" spans="1:4" x14ac:dyDescent="0.45">
@@ -24924,10 +24937,10 @@
         <v>313</v>
       </c>
       <c r="C807" s="13">
-        <v>5155</v>
+        <v>5154</v>
       </c>
       <c r="D807" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="808" spans="1:4" x14ac:dyDescent="0.45">
@@ -24937,11 +24950,11 @@
       <c r="B808" t="s">
         <v>313</v>
       </c>
-      <c r="C808" s="34">
-        <v>5156</v>
-      </c>
-      <c r="D808" s="29" t="s">
-        <v>1387</v>
+      <c r="C808" s="13">
+        <v>5155</v>
+      </c>
+      <c r="D808" t="s">
+        <v>1386</v>
       </c>
     </row>
     <row r="809" spans="1:4" x14ac:dyDescent="0.45">
@@ -24952,10 +24965,10 @@
         <v>313</v>
       </c>
       <c r="C809" s="34">
-        <v>5157</v>
+        <v>5156</v>
       </c>
       <c r="D809" s="29" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="810" spans="1:4" x14ac:dyDescent="0.45">
@@ -24966,10 +24979,10 @@
         <v>313</v>
       </c>
       <c r="C810" s="34">
-        <v>5158</v>
+        <v>5157</v>
       </c>
       <c r="D810" s="29" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="811" spans="1:4" x14ac:dyDescent="0.45">
@@ -24980,10 +24993,10 @@
         <v>313</v>
       </c>
       <c r="C811" s="34">
-        <v>5159</v>
+        <v>5158</v>
       </c>
       <c r="D811" s="29" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="812" spans="1:4" x14ac:dyDescent="0.45">
@@ -24994,10 +25007,10 @@
         <v>313</v>
       </c>
       <c r="C812" s="34">
-        <v>5160</v>
+        <v>5159</v>
       </c>
       <c r="D812" s="29" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="813" spans="1:4" x14ac:dyDescent="0.45">
@@ -25008,10 +25021,10 @@
         <v>313</v>
       </c>
       <c r="C813" s="34">
-        <v>5161</v>
+        <v>5160</v>
       </c>
       <c r="D813" s="29" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="814" spans="1:4" x14ac:dyDescent="0.45">
@@ -25022,10 +25035,10 @@
         <v>313</v>
       </c>
       <c r="C814" s="34">
-        <v>5162</v>
+        <v>5161</v>
       </c>
       <c r="D814" s="29" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="815" spans="1:4" x14ac:dyDescent="0.45">
@@ -25036,10 +25049,10 @@
         <v>313</v>
       </c>
       <c r="C815" s="34">
-        <v>5163</v>
+        <v>5162</v>
       </c>
       <c r="D815" s="29" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="816" spans="1:4" x14ac:dyDescent="0.45">
@@ -25050,10 +25063,10 @@
         <v>313</v>
       </c>
       <c r="C816" s="34">
-        <v>5164</v>
+        <v>5163</v>
       </c>
       <c r="D816" s="29" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="817" spans="1:4" x14ac:dyDescent="0.45">
@@ -25064,10 +25077,10 @@
         <v>313</v>
       </c>
       <c r="C817" s="34">
-        <v>5165</v>
+        <v>5164</v>
       </c>
       <c r="D817" s="29" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="818" spans="1:4" x14ac:dyDescent="0.45">
@@ -25078,10 +25091,10 @@
         <v>313</v>
       </c>
       <c r="C818" s="34">
-        <v>5166</v>
+        <v>5165</v>
       </c>
       <c r="D818" s="29" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="819" spans="1:4" x14ac:dyDescent="0.45">
@@ -25092,10 +25105,10 @@
         <v>313</v>
       </c>
       <c r="C819" s="34">
-        <v>5167</v>
+        <v>5166</v>
       </c>
       <c r="D819" s="29" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="820" spans="1:4" x14ac:dyDescent="0.45">
@@ -25106,10 +25119,10 @@
         <v>313</v>
       </c>
       <c r="C820" s="34">
-        <v>5168</v>
+        <v>5167</v>
       </c>
       <c r="D820" s="29" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="821" spans="1:4" x14ac:dyDescent="0.45">
@@ -25120,10 +25133,10 @@
         <v>313</v>
       </c>
       <c r="C821" s="34">
-        <v>5169</v>
+        <v>5168</v>
       </c>
       <c r="D821" s="29" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="822" spans="1:4" x14ac:dyDescent="0.45">
@@ -25134,10 +25147,10 @@
         <v>313</v>
       </c>
       <c r="C822" s="34">
-        <v>5170</v>
+        <v>5169</v>
       </c>
       <c r="D822" s="29" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="823" spans="1:4" x14ac:dyDescent="0.45">
@@ -25148,10 +25161,10 @@
         <v>313</v>
       </c>
       <c r="C823" s="34">
-        <v>5171</v>
+        <v>5170</v>
       </c>
       <c r="D823" s="29" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="824" spans="1:4" x14ac:dyDescent="0.45">
@@ -25162,10 +25175,10 @@
         <v>313</v>
       </c>
       <c r="C824" s="34">
-        <v>5172</v>
+        <v>5171</v>
       </c>
       <c r="D824" s="29" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="825" spans="1:4" x14ac:dyDescent="0.45">
@@ -25176,10 +25189,10 @@
         <v>313</v>
       </c>
       <c r="C825" s="34">
-        <v>5173</v>
+        <v>5172</v>
       </c>
       <c r="D825" s="29" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="826" spans="1:4" x14ac:dyDescent="0.45">
@@ -25190,10 +25203,10 @@
         <v>313</v>
       </c>
       <c r="C826" s="34">
-        <v>5174</v>
+        <v>5173</v>
       </c>
       <c r="D826" s="29" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="827" spans="1:4" x14ac:dyDescent="0.45">
@@ -25204,10 +25217,10 @@
         <v>313</v>
       </c>
       <c r="C827" s="34">
-        <v>5175</v>
+        <v>5174</v>
       </c>
       <c r="D827" s="29" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="828" spans="1:4" x14ac:dyDescent="0.45">
@@ -25218,10 +25231,10 @@
         <v>313</v>
       </c>
       <c r="C828" s="34">
-        <v>5176</v>
+        <v>5175</v>
       </c>
       <c r="D828" s="29" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="829" spans="1:4" x14ac:dyDescent="0.45">
@@ -25232,10 +25245,10 @@
         <v>313</v>
       </c>
       <c r="C829" s="34">
-        <v>5177</v>
+        <v>5176</v>
       </c>
       <c r="D829" s="29" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="830" spans="1:4" x14ac:dyDescent="0.45">
@@ -25246,10 +25259,10 @@
         <v>313</v>
       </c>
       <c r="C830" s="34">
-        <v>5178</v>
+        <v>5177</v>
       </c>
       <c r="D830" s="29" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="831" spans="1:4" x14ac:dyDescent="0.45">
@@ -25260,10 +25273,10 @@
         <v>313</v>
       </c>
       <c r="C831" s="34">
-        <v>5179</v>
+        <v>5178</v>
       </c>
       <c r="D831" s="29" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="832" spans="1:4" x14ac:dyDescent="0.45">
@@ -25274,10 +25287,10 @@
         <v>313</v>
       </c>
       <c r="C832" s="34">
-        <v>5180</v>
+        <v>5179</v>
       </c>
       <c r="D832" s="29" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="833" spans="1:4" x14ac:dyDescent="0.45">
@@ -25288,10 +25301,10 @@
         <v>313</v>
       </c>
       <c r="C833" s="34">
-        <v>5181</v>
+        <v>5180</v>
       </c>
       <c r="D833" s="29" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="834" spans="1:4" x14ac:dyDescent="0.45">
@@ -25302,10 +25315,10 @@
         <v>313</v>
       </c>
       <c r="C834" s="34">
-        <v>5182</v>
+        <v>5181</v>
       </c>
       <c r="D834" s="29" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="835" spans="1:4" x14ac:dyDescent="0.45">
@@ -25316,10 +25329,10 @@
         <v>313</v>
       </c>
       <c r="C835" s="34">
-        <v>5183</v>
+        <v>5182</v>
       </c>
       <c r="D835" s="29" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="836" spans="1:4" x14ac:dyDescent="0.45">
@@ -25330,10 +25343,10 @@
         <v>313</v>
       </c>
       <c r="C836" s="34">
-        <v>5184</v>
+        <v>5183</v>
       </c>
       <c r="D836" s="29" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="837" spans="1:4" x14ac:dyDescent="0.45">
@@ -25344,10 +25357,10 @@
         <v>313</v>
       </c>
       <c r="C837" s="34">
-        <v>5185</v>
+        <v>5184</v>
       </c>
       <c r="D837" s="29" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="838" spans="1:4" x14ac:dyDescent="0.45">
@@ -25357,11 +25370,11 @@
       <c r="B838" t="s">
         <v>313</v>
       </c>
-      <c r="C838" s="13">
-        <v>5253</v>
-      </c>
-      <c r="D838" t="s">
-        <v>1417</v>
+      <c r="C838" s="34">
+        <v>5185</v>
+      </c>
+      <c r="D838" s="29" t="s">
+        <v>1416</v>
       </c>
     </row>
     <row r="839" spans="1:4" x14ac:dyDescent="0.45">
@@ -25371,11 +25384,11 @@
       <c r="B839" t="s">
         <v>313</v>
       </c>
-      <c r="C839" s="13">
-        <v>5254</v>
-      </c>
-      <c r="D839" t="s">
-        <v>1418</v>
+      <c r="C839" s="34">
+        <v>5197</v>
+      </c>
+      <c r="D839" s="29" t="s">
+        <v>1564</v>
       </c>
     </row>
     <row r="840" spans="1:4" x14ac:dyDescent="0.45">
@@ -25386,10 +25399,10 @@
         <v>313</v>
       </c>
       <c r="C840" s="13">
-        <v>5255</v>
+        <v>5253</v>
       </c>
       <c r="D840" t="s">
-        <v>392</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="841" spans="1:4" x14ac:dyDescent="0.45">
@@ -25399,11 +25412,11 @@
       <c r="B841" t="s">
         <v>313</v>
       </c>
-      <c r="C841" s="34">
-        <v>5256</v>
-      </c>
-      <c r="D841" s="29" t="s">
-        <v>1419</v>
+      <c r="C841" s="13">
+        <v>5254</v>
+      </c>
+      <c r="D841" t="s">
+        <v>1418</v>
       </c>
     </row>
     <row r="842" spans="1:4" x14ac:dyDescent="0.45">
@@ -25413,11 +25426,11 @@
       <c r="B842" t="s">
         <v>313</v>
       </c>
-      <c r="C842" s="34">
-        <v>5257</v>
-      </c>
-      <c r="D842" s="29" t="s">
-        <v>1420</v>
+      <c r="C842" s="13">
+        <v>5255</v>
+      </c>
+      <c r="D842" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="843" spans="1:4" x14ac:dyDescent="0.45">
@@ -25428,10 +25441,10 @@
         <v>313</v>
       </c>
       <c r="C843" s="34">
-        <v>5258</v>
+        <v>5256</v>
       </c>
       <c r="D843" s="29" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="844" spans="1:4" x14ac:dyDescent="0.45">
@@ -25442,10 +25455,10 @@
         <v>313</v>
       </c>
       <c r="C844" s="34">
-        <v>5259</v>
+        <v>5257</v>
       </c>
       <c r="D844" s="29" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="845" spans="1:4" x14ac:dyDescent="0.45">
@@ -25456,10 +25469,10 @@
         <v>313</v>
       </c>
       <c r="C845" s="34">
-        <v>5260</v>
+        <v>5258</v>
       </c>
       <c r="D845" s="29" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="846" spans="1:4" x14ac:dyDescent="0.45">
@@ -25470,10 +25483,10 @@
         <v>313</v>
       </c>
       <c r="C846" s="34">
-        <v>5261</v>
+        <v>5259</v>
       </c>
       <c r="D846" s="29" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="847" spans="1:4" x14ac:dyDescent="0.45">
@@ -25484,10 +25497,10 @@
         <v>313</v>
       </c>
       <c r="C847" s="34">
-        <v>5262</v>
+        <v>5260</v>
       </c>
       <c r="D847" s="29" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="848" spans="1:4" x14ac:dyDescent="0.45">
@@ -25498,10 +25511,10 @@
         <v>313</v>
       </c>
       <c r="C848" s="34">
-        <v>5263</v>
+        <v>5261</v>
       </c>
       <c r="D848" s="29" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="849" spans="1:4" x14ac:dyDescent="0.45">
@@ -25512,10 +25525,10 @@
         <v>313</v>
       </c>
       <c r="C849" s="34">
-        <v>5264</v>
+        <v>5262</v>
       </c>
       <c r="D849" s="29" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="850" spans="1:4" x14ac:dyDescent="0.45">
@@ -25526,10 +25539,10 @@
         <v>313</v>
       </c>
       <c r="C850" s="34">
-        <v>5265</v>
+        <v>5263</v>
       </c>
       <c r="D850" s="29" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="851" spans="1:4" x14ac:dyDescent="0.45">
@@ -25540,10 +25553,10 @@
         <v>313</v>
       </c>
       <c r="C851" s="34">
-        <v>5266</v>
+        <v>5264</v>
       </c>
       <c r="D851" s="29" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="852" spans="1:4" x14ac:dyDescent="0.45">
@@ -25554,10 +25567,10 @@
         <v>313</v>
       </c>
       <c r="C852" s="34">
-        <v>5267</v>
+        <v>5265</v>
       </c>
       <c r="D852" s="29" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="853" spans="1:4" x14ac:dyDescent="0.45">
@@ -25568,10 +25581,10 @@
         <v>313</v>
       </c>
       <c r="C853" s="34">
-        <v>5268</v>
+        <v>5266</v>
       </c>
       <c r="D853" s="29" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="854" spans="1:4" x14ac:dyDescent="0.45">
@@ -25582,10 +25595,10 @@
         <v>313</v>
       </c>
       <c r="C854" s="34">
-        <v>5269</v>
+        <v>5267</v>
       </c>
       <c r="D854" s="29" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="855" spans="1:4" x14ac:dyDescent="0.45">
@@ -25596,10 +25609,10 @@
         <v>313</v>
       </c>
       <c r="C855" s="34">
-        <v>5270</v>
+        <v>5268</v>
       </c>
       <c r="D855" s="29" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="856" spans="1:4" x14ac:dyDescent="0.45">
@@ -25610,10 +25623,10 @@
         <v>313</v>
       </c>
       <c r="C856" s="34">
-        <v>5271</v>
+        <v>5269</v>
       </c>
       <c r="D856" s="29" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="857" spans="1:4" x14ac:dyDescent="0.45">
@@ -25624,10 +25637,10 @@
         <v>313</v>
       </c>
       <c r="C857" s="34">
-        <v>5272</v>
+        <v>5270</v>
       </c>
       <c r="D857" s="29" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="858" spans="1:4" x14ac:dyDescent="0.45">
@@ -25638,10 +25651,10 @@
         <v>313</v>
       </c>
       <c r="C858" s="34">
-        <v>5273</v>
+        <v>5271</v>
       </c>
       <c r="D858" s="29" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="859" spans="1:4" x14ac:dyDescent="0.45">
@@ -25652,10 +25665,10 @@
         <v>313</v>
       </c>
       <c r="C859" s="34">
-        <v>5274</v>
+        <v>5272</v>
       </c>
       <c r="D859" s="29" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="860" spans="1:4" x14ac:dyDescent="0.45">
@@ -25666,10 +25679,10 @@
         <v>313</v>
       </c>
       <c r="C860" s="34">
-        <v>5275</v>
+        <v>5273</v>
       </c>
       <c r="D860" s="29" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="861" spans="1:4" x14ac:dyDescent="0.45">
@@ -25680,10 +25693,10 @@
         <v>313</v>
       </c>
       <c r="C861" s="34">
-        <v>5276</v>
+        <v>5274</v>
       </c>
       <c r="D861" s="29" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="862" spans="1:4" x14ac:dyDescent="0.45">
@@ -25694,10 +25707,10 @@
         <v>313</v>
       </c>
       <c r="C862" s="34">
-        <v>5277</v>
+        <v>5275</v>
       </c>
       <c r="D862" s="29" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="863" spans="1:4" x14ac:dyDescent="0.45">
@@ -25708,10 +25721,10 @@
         <v>313</v>
       </c>
       <c r="C863" s="34">
-        <v>5278</v>
+        <v>5276</v>
       </c>
       <c r="D863" s="29" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="864" spans="1:4" x14ac:dyDescent="0.45">
@@ -25722,10 +25735,10 @@
         <v>313</v>
       </c>
       <c r="C864" s="34">
-        <v>5279</v>
+        <v>5277</v>
       </c>
       <c r="D864" s="29" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="865" spans="1:4" x14ac:dyDescent="0.45">
@@ -25736,10 +25749,10 @@
         <v>313</v>
       </c>
       <c r="C865" s="34">
-        <v>5280</v>
+        <v>5278</v>
       </c>
       <c r="D865" s="29" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="866" spans="1:4" x14ac:dyDescent="0.45">
@@ -25750,10 +25763,10 @@
         <v>313</v>
       </c>
       <c r="C866" s="34">
-        <v>5281</v>
+        <v>5279</v>
       </c>
       <c r="D866" s="29" t="s">
-        <v>391</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="867" spans="1:4" x14ac:dyDescent="0.45">
@@ -25764,10 +25777,10 @@
         <v>313</v>
       </c>
       <c r="C867" s="34">
-        <v>5282</v>
+        <v>5280</v>
       </c>
       <c r="D867" s="29" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="868" spans="1:4" x14ac:dyDescent="0.45">
@@ -25778,10 +25791,10 @@
         <v>313</v>
       </c>
       <c r="C868" s="34">
-        <v>5283</v>
+        <v>5281</v>
       </c>
       <c r="D868" s="29" t="s">
-        <v>434</v>
+        <v>391</v>
       </c>
     </row>
     <row r="869" spans="1:4" x14ac:dyDescent="0.45">
@@ -25792,10 +25805,10 @@
         <v>313</v>
       </c>
       <c r="C869" s="34">
-        <v>5284</v>
+        <v>5282</v>
       </c>
       <c r="D869" s="29" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="870" spans="1:4" x14ac:dyDescent="0.45">
@@ -25806,10 +25819,10 @@
         <v>313</v>
       </c>
       <c r="C870" s="34">
-        <v>5285</v>
+        <v>5283</v>
       </c>
       <c r="D870" s="29" t="s">
-        <v>1446</v>
+        <v>434</v>
       </c>
     </row>
     <row r="871" spans="1:4" x14ac:dyDescent="0.45">
@@ -25819,11 +25832,11 @@
       <c r="B871" t="s">
         <v>313</v>
       </c>
-      <c r="C871" s="13">
-        <v>5253</v>
-      </c>
-      <c r="D871" t="s">
-        <v>428</v>
+      <c r="C871" s="34">
+        <v>5284</v>
+      </c>
+      <c r="D871" s="29" t="s">
+        <v>1445</v>
       </c>
     </row>
     <row r="872" spans="1:4" x14ac:dyDescent="0.45">
@@ -25833,11 +25846,11 @@
       <c r="B872" t="s">
         <v>313</v>
       </c>
-      <c r="C872" s="13">
-        <v>5254</v>
-      </c>
-      <c r="D872" t="s">
-        <v>429</v>
+      <c r="C872" s="34">
+        <v>5285</v>
+      </c>
+      <c r="D872" s="29" t="s">
+        <v>1446</v>
       </c>
     </row>
     <row r="873" spans="1:4" x14ac:dyDescent="0.45">
@@ -25848,10 +25861,10 @@
         <v>313</v>
       </c>
       <c r="C873" s="13">
-        <v>5255</v>
+        <v>5253</v>
       </c>
       <c r="D873" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
     </row>
     <row r="874" spans="1:4" x14ac:dyDescent="0.45">
@@ -25861,11 +25874,11 @@
       <c r="B874" t="s">
         <v>313</v>
       </c>
-      <c r="C874" s="34">
-        <v>5256</v>
-      </c>
-      <c r="D874" s="29" t="s">
-        <v>1135</v>
+      <c r="C874" s="13">
+        <v>5254</v>
+      </c>
+      <c r="D874" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="875" spans="1:4" x14ac:dyDescent="0.45">
@@ -25875,11 +25888,11 @@
       <c r="B875" t="s">
         <v>313</v>
       </c>
-      <c r="C875" s="34">
-        <v>5257</v>
-      </c>
-      <c r="D875" s="29" t="s">
-        <v>1136</v>
+      <c r="C875" s="13">
+        <v>5255</v>
+      </c>
+      <c r="D875" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="876" spans="1:4" x14ac:dyDescent="0.45">
@@ -25890,10 +25903,10 @@
         <v>313</v>
       </c>
       <c r="C876" s="34">
-        <v>5258</v>
+        <v>5256</v>
       </c>
       <c r="D876" s="29" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="877" spans="1:4" x14ac:dyDescent="0.45">
@@ -25904,10 +25917,10 @@
         <v>313</v>
       </c>
       <c r="C877" s="34">
-        <v>5259</v>
+        <v>5257</v>
       </c>
       <c r="D877" s="29" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="878" spans="1:4" x14ac:dyDescent="0.45">
@@ -25918,10 +25931,10 @@
         <v>313</v>
       </c>
       <c r="C878" s="34">
-        <v>5260</v>
+        <v>5258</v>
       </c>
       <c r="D878" s="29" t="s">
-        <v>430</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="879" spans="1:4" x14ac:dyDescent="0.45">
@@ -25932,10 +25945,10 @@
         <v>313</v>
       </c>
       <c r="C879" s="34">
-        <v>5261</v>
+        <v>5259</v>
       </c>
       <c r="D879" s="29" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="880" spans="1:4" x14ac:dyDescent="0.45">
@@ -25946,10 +25959,10 @@
         <v>313</v>
       </c>
       <c r="C880" s="34">
-        <v>5262</v>
+        <v>5260</v>
       </c>
       <c r="D880" s="29" t="s">
-        <v>1140</v>
+        <v>430</v>
       </c>
     </row>
     <row r="881" spans="1:4" x14ac:dyDescent="0.45">
@@ -25960,10 +25973,10 @@
         <v>313</v>
       </c>
       <c r="C881" s="34">
-        <v>5263</v>
+        <v>5261</v>
       </c>
       <c r="D881" s="29" t="s">
-        <v>431</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="882" spans="1:4" x14ac:dyDescent="0.45">
@@ -25974,10 +25987,10 @@
         <v>313</v>
       </c>
       <c r="C882" s="34">
-        <v>5264</v>
+        <v>5262</v>
       </c>
       <c r="D882" s="29" t="s">
-        <v>432</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="883" spans="1:4" x14ac:dyDescent="0.45">
@@ -25988,10 +26001,10 @@
         <v>313</v>
       </c>
       <c r="C883" s="34">
-        <v>5265</v>
+        <v>5263</v>
       </c>
       <c r="D883" s="29" t="s">
-        <v>1141</v>
+        <v>431</v>
       </c>
     </row>
     <row r="884" spans="1:4" x14ac:dyDescent="0.45">
@@ -26002,10 +26015,10 @@
         <v>313</v>
       </c>
       <c r="C884" s="34">
-        <v>5266</v>
+        <v>5264</v>
       </c>
       <c r="D884" s="29" t="s">
-        <v>1142</v>
+        <v>432</v>
       </c>
     </row>
     <row r="885" spans="1:4" x14ac:dyDescent="0.45">
@@ -26016,10 +26029,10 @@
         <v>313</v>
       </c>
       <c r="C885" s="34">
-        <v>5267</v>
+        <v>5265</v>
       </c>
       <c r="D885" s="29" t="s">
-        <v>389</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="886" spans="1:4" x14ac:dyDescent="0.45">
@@ -26030,10 +26043,10 @@
         <v>313</v>
       </c>
       <c r="C886" s="34">
-        <v>5268</v>
+        <v>5266</v>
       </c>
       <c r="D886" s="29" t="s">
-        <v>390</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="887" spans="1:4" x14ac:dyDescent="0.45">
@@ -26044,10 +26057,10 @@
         <v>313</v>
       </c>
       <c r="C887" s="34">
-        <v>5269</v>
+        <v>5267</v>
       </c>
       <c r="D887" s="29" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="888" spans="1:4" x14ac:dyDescent="0.45">
@@ -26058,10 +26071,10 @@
         <v>313</v>
       </c>
       <c r="C888" s="34">
-        <v>5270</v>
+        <v>5268</v>
       </c>
       <c r="D888" s="29" t="s">
-        <v>433</v>
+        <v>390</v>
       </c>
     </row>
     <row r="889" spans="1:4" x14ac:dyDescent="0.45">
@@ -26072,52 +26085,52 @@
         <v>313</v>
       </c>
       <c r="C889" s="34">
-        <v>5271</v>
+        <v>5269</v>
       </c>
       <c r="D889" s="29" t="s">
-        <v>434</v>
+        <v>391</v>
       </c>
     </row>
     <row r="890" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A890">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B890" t="s">
-        <v>316</v>
-      </c>
-      <c r="C890">
-        <v>1</v>
-      </c>
-      <c r="D890" t="s">
-        <v>435</v>
+        <v>313</v>
+      </c>
+      <c r="C890" s="34">
+        <v>5270</v>
+      </c>
+      <c r="D890" s="29" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="891" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A891">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B891" t="s">
-        <v>316</v>
-      </c>
-      <c r="C891">
-        <v>2</v>
-      </c>
-      <c r="D891" t="s">
-        <v>436</v>
+        <v>313</v>
+      </c>
+      <c r="C891" s="34">
+        <v>5271</v>
+      </c>
+      <c r="D891" s="29" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="892" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A892">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B892" t="s">
-        <v>316</v>
-      </c>
-      <c r="C892">
-        <v>3</v>
-      </c>
-      <c r="D892" t="s">
-        <v>437</v>
+        <v>313</v>
+      </c>
+      <c r="C892" s="34">
+        <v>5291</v>
+      </c>
+      <c r="D892" s="29" t="s">
+        <v>1565</v>
       </c>
     </row>
     <row r="893" spans="1:4" x14ac:dyDescent="0.45">
@@ -26128,10 +26141,10 @@
         <v>316</v>
       </c>
       <c r="C893">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D893" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="894" spans="1:4" x14ac:dyDescent="0.45">
@@ -26142,10 +26155,10 @@
         <v>316</v>
       </c>
       <c r="C894">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D894" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="895" spans="1:4" x14ac:dyDescent="0.45">
@@ -26156,10 +26169,10 @@
         <v>316</v>
       </c>
       <c r="C895">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D895" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="896" spans="1:4" x14ac:dyDescent="0.45">
@@ -26170,10 +26183,10 @@
         <v>316</v>
       </c>
       <c r="C896">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D896" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="897" spans="1:4" x14ac:dyDescent="0.45">
@@ -26184,10 +26197,10 @@
         <v>316</v>
       </c>
       <c r="C897">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D897" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="898" spans="1:4" x14ac:dyDescent="0.45">
@@ -26198,10 +26211,10 @@
         <v>316</v>
       </c>
       <c r="C898">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D898" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="899" spans="1:4" x14ac:dyDescent="0.45">
@@ -26212,10 +26225,10 @@
         <v>316</v>
       </c>
       <c r="C899">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D899" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="900" spans="1:4" x14ac:dyDescent="0.45">
@@ -26226,10 +26239,10 @@
         <v>316</v>
       </c>
       <c r="C900">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D900" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="901" spans="1:4" x14ac:dyDescent="0.45">
@@ -26240,10 +26253,10 @@
         <v>316</v>
       </c>
       <c r="C901">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D901" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="902" spans="1:4" x14ac:dyDescent="0.45">
@@ -26254,10 +26267,10 @@
         <v>316</v>
       </c>
       <c r="C902">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D902" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="903" spans="1:4" x14ac:dyDescent="0.45">
@@ -26268,10 +26281,10 @@
         <v>316</v>
       </c>
       <c r="C903">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D903" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="904" spans="1:4" x14ac:dyDescent="0.45">
@@ -26282,10 +26295,10 @@
         <v>316</v>
       </c>
       <c r="C904">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D904" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="905" spans="1:4" x14ac:dyDescent="0.45">
@@ -26296,10 +26309,10 @@
         <v>316</v>
       </c>
       <c r="C905">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D905" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="906" spans="1:4" x14ac:dyDescent="0.45">
@@ -26310,10 +26323,10 @@
         <v>316</v>
       </c>
       <c r="C906">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D906" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="907" spans="1:4" x14ac:dyDescent="0.45">
@@ -26324,10 +26337,10 @@
         <v>316</v>
       </c>
       <c r="C907">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D907" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="908" spans="1:4" x14ac:dyDescent="0.45">
@@ -26338,10 +26351,10 @@
         <v>316</v>
       </c>
       <c r="C908">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D908" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="909" spans="1:4" x14ac:dyDescent="0.45">
@@ -26352,10 +26365,10 @@
         <v>316</v>
       </c>
       <c r="C909">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D909" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="910" spans="1:4" x14ac:dyDescent="0.45">
@@ -26366,10 +26379,10 @@
         <v>316</v>
       </c>
       <c r="C910">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D910" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="911" spans="1:4" x14ac:dyDescent="0.45">
@@ -26380,10 +26393,10 @@
         <v>316</v>
       </c>
       <c r="C911">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D911" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="912" spans="1:4" x14ac:dyDescent="0.45">
@@ -26394,10 +26407,10 @@
         <v>316</v>
       </c>
       <c r="C912">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D912" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="913" spans="1:4" x14ac:dyDescent="0.45">
@@ -26408,10 +26421,10 @@
         <v>316</v>
       </c>
       <c r="C913">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D913" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="914" spans="1:4" x14ac:dyDescent="0.45">
@@ -26422,10 +26435,10 @@
         <v>316</v>
       </c>
       <c r="C914">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D914" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="915" spans="1:4" x14ac:dyDescent="0.45">
@@ -26436,10 +26449,10 @@
         <v>316</v>
       </c>
       <c r="C915">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D915" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="916" spans="1:4" x14ac:dyDescent="0.45">
@@ -26450,10 +26463,10 @@
         <v>316</v>
       </c>
       <c r="C916">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D916" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="917" spans="1:4" x14ac:dyDescent="0.45">
@@ -26464,10 +26477,10 @@
         <v>316</v>
       </c>
       <c r="C917">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D917" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="918" spans="1:4" x14ac:dyDescent="0.45">
@@ -26478,10 +26491,10 @@
         <v>316</v>
       </c>
       <c r="C918">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D918" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="919" spans="1:4" x14ac:dyDescent="0.45">
@@ -26492,10 +26505,10 @@
         <v>316</v>
       </c>
       <c r="C919">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D919" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="920" spans="1:4" x14ac:dyDescent="0.45">
@@ -26506,10 +26519,10 @@
         <v>316</v>
       </c>
       <c r="C920">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D920" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="921" spans="1:4" x14ac:dyDescent="0.45">
@@ -26520,10 +26533,10 @@
         <v>316</v>
       </c>
       <c r="C921">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D921" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="922" spans="1:4" x14ac:dyDescent="0.45">
@@ -26534,10 +26547,10 @@
         <v>316</v>
       </c>
       <c r="C922">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D922" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="923" spans="1:4" x14ac:dyDescent="0.45">
@@ -26548,10 +26561,10 @@
         <v>316</v>
       </c>
       <c r="C923">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D923" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="924" spans="1:4" x14ac:dyDescent="0.45">
@@ -26562,10 +26575,10 @@
         <v>316</v>
       </c>
       <c r="C924">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D924" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="925" spans="1:4" x14ac:dyDescent="0.45">
@@ -26576,10 +26589,10 @@
         <v>316</v>
       </c>
       <c r="C925">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="D925" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="926" spans="1:4" x14ac:dyDescent="0.45">
@@ -26590,10 +26603,10 @@
         <v>316</v>
       </c>
       <c r="C926">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D926" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="927" spans="1:4" x14ac:dyDescent="0.45">
@@ -26604,10 +26617,10 @@
         <v>316</v>
       </c>
       <c r="C927">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D927" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="928" spans="1:4" x14ac:dyDescent="0.45">
@@ -26618,10 +26631,10 @@
         <v>316</v>
       </c>
       <c r="C928">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D928" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="929" spans="1:4" x14ac:dyDescent="0.45">
@@ -26632,10 +26645,10 @@
         <v>316</v>
       </c>
       <c r="C929">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D929" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="930" spans="1:4" x14ac:dyDescent="0.45">
@@ -26646,10 +26659,10 @@
         <v>316</v>
       </c>
       <c r="C930">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D930" t="s">
-        <v>675</v>
+        <v>472</v>
       </c>
     </row>
     <row r="931" spans="1:4" x14ac:dyDescent="0.45">
@@ -26660,52 +26673,52 @@
         <v>316</v>
       </c>
       <c r="C931">
+        <v>56</v>
+      </c>
+      <c r="D931" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="932" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A932">
+        <v>33</v>
+      </c>
+      <c r="B932" t="s">
+        <v>316</v>
+      </c>
+      <c r="C932">
+        <v>57</v>
+      </c>
+      <c r="D932" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="933" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A933">
+        <v>33</v>
+      </c>
+      <c r="B933" t="s">
+        <v>316</v>
+      </c>
+      <c r="C933">
+        <v>63</v>
+      </c>
+      <c r="D933" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="934" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A934">
+        <v>33</v>
+      </c>
+      <c r="B934" t="s">
+        <v>316</v>
+      </c>
+      <c r="C934">
         <v>64</v>
       </c>
-      <c r="D931" t="s">
+      <c r="D934" t="s">
         <v>676</v>
-      </c>
-    </row>
-    <row r="932" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A932" s="29">
-        <v>33</v>
-      </c>
-      <c r="B932" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="C932" s="29">
-        <v>65</v>
-      </c>
-      <c r="D932" s="29" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="933" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A933" s="29">
-        <v>33</v>
-      </c>
-      <c r="B933" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="C933" s="29">
-        <v>66</v>
-      </c>
-      <c r="D933" s="29" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="934" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A934" s="29">
-        <v>33</v>
-      </c>
-      <c r="B934" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="C934" s="29">
-        <v>101</v>
-      </c>
-      <c r="D934" s="29" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="935" spans="1:4" x14ac:dyDescent="0.45">
@@ -26716,10 +26729,10 @@
         <v>316</v>
       </c>
       <c r="C935" s="29">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="D935" s="29" t="s">
-        <v>1470</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="936" spans="1:4" x14ac:dyDescent="0.45">
@@ -26730,10 +26743,10 @@
         <v>316</v>
       </c>
       <c r="C936" s="29">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="D936" s="29" t="s">
-        <v>1471</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="937" spans="1:4" x14ac:dyDescent="0.45">
@@ -26744,10 +26757,10 @@
         <v>316</v>
       </c>
       <c r="C937" s="29">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D937" s="29" t="s">
-        <v>1472</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="938" spans="1:4" x14ac:dyDescent="0.45">
@@ -26758,10 +26771,10 @@
         <v>316</v>
       </c>
       <c r="C938" s="29">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D938" s="29" t="s">
-        <v>1473</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="939" spans="1:4" x14ac:dyDescent="0.45">
@@ -26772,10 +26785,10 @@
         <v>316</v>
       </c>
       <c r="C939" s="29">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D939" s="29" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="940" spans="1:4" x14ac:dyDescent="0.45">
@@ -26786,10 +26799,10 @@
         <v>316</v>
       </c>
       <c r="C940" s="29">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D940" s="29" t="s">
-        <v>1475</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="941" spans="1:4" x14ac:dyDescent="0.45">
@@ -26800,10 +26813,10 @@
         <v>316</v>
       </c>
       <c r="C941" s="29">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D941" s="29" t="s">
-        <v>1476</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="942" spans="1:4" x14ac:dyDescent="0.45">
@@ -26814,10 +26827,10 @@
         <v>316</v>
       </c>
       <c r="C942" s="29">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D942" s="29" t="s">
-        <v>1477</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="943" spans="1:4" x14ac:dyDescent="0.45">
@@ -26828,10 +26841,10 @@
         <v>316</v>
       </c>
       <c r="C943" s="29">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D943" s="29" t="s">
-        <v>1478</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="944" spans="1:4" x14ac:dyDescent="0.45">
@@ -26842,10 +26855,10 @@
         <v>316</v>
       </c>
       <c r="C944" s="29">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D944" s="29" t="s">
-        <v>1479</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="945" spans="1:4" x14ac:dyDescent="0.45">
@@ -26856,10 +26869,10 @@
         <v>316</v>
       </c>
       <c r="C945" s="29">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D945" s="29" t="s">
-        <v>1480</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="946" spans="1:4" x14ac:dyDescent="0.45">
@@ -26870,10 +26883,10 @@
         <v>316</v>
       </c>
       <c r="C946" s="29">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D946" s="29" t="s">
-        <v>1481</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="947" spans="1:4" x14ac:dyDescent="0.45">
@@ -26884,10 +26897,10 @@
         <v>316</v>
       </c>
       <c r="C947" s="29">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D947" s="29" t="s">
-        <v>1482</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="948" spans="1:4" x14ac:dyDescent="0.45">
@@ -26898,10 +26911,10 @@
         <v>316</v>
       </c>
       <c r="C948" s="29">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D948" s="29" t="s">
-        <v>1483</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="949" spans="1:4" x14ac:dyDescent="0.45">
@@ -26912,10 +26925,10 @@
         <v>316</v>
       </c>
       <c r="C949" s="29">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D949" s="29" t="s">
-        <v>1484</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="950" spans="1:4" x14ac:dyDescent="0.45">
@@ -26926,10 +26939,10 @@
         <v>316</v>
       </c>
       <c r="C950" s="29">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D950" s="29" t="s">
-        <v>1485</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="951" spans="1:4" x14ac:dyDescent="0.45">
@@ -26940,10 +26953,10 @@
         <v>316</v>
       </c>
       <c r="C951" s="29">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D951" s="29" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="952" spans="1:4" x14ac:dyDescent="0.45">
@@ -26954,10 +26967,10 @@
         <v>316</v>
       </c>
       <c r="C952" s="29">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D952" s="29" t="s">
-        <v>1504</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="953" spans="1:4" x14ac:dyDescent="0.45">
@@ -26968,10 +26981,10 @@
         <v>316</v>
       </c>
       <c r="C953" s="29">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D953" s="29" t="s">
-        <v>1505</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="954" spans="1:4" x14ac:dyDescent="0.45">
@@ -26982,10 +26995,10 @@
         <v>316</v>
       </c>
       <c r="C954" s="29">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D954" s="29" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="955" spans="1:4" x14ac:dyDescent="0.45">
@@ -26996,10 +27009,10 @@
         <v>316</v>
       </c>
       <c r="C955" s="29">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D955" s="29" t="s">
-        <v>1489</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="956" spans="1:4" x14ac:dyDescent="0.45">
@@ -27010,10 +27023,10 @@
         <v>316</v>
       </c>
       <c r="C956" s="29">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D956" s="29" t="s">
-        <v>1490</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="957" spans="1:4" x14ac:dyDescent="0.45">
@@ -27024,10 +27037,10 @@
         <v>316</v>
       </c>
       <c r="C957" s="29">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D957" s="29" t="s">
-        <v>1491</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="958" spans="1:4" x14ac:dyDescent="0.45">
@@ -27038,10 +27051,10 @@
         <v>316</v>
       </c>
       <c r="C958" s="29">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D958" s="29" t="s">
-        <v>1506</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="959" spans="1:4" x14ac:dyDescent="0.45">
@@ -27052,10 +27065,10 @@
         <v>316</v>
       </c>
       <c r="C959" s="29">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D959" s="29" t="s">
-        <v>1507</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="960" spans="1:4" x14ac:dyDescent="0.45">
@@ -27066,10 +27079,10 @@
         <v>316</v>
       </c>
       <c r="C960" s="29">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D960" s="29" t="s">
-        <v>1508</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.45">
@@ -27080,10 +27093,10 @@
         <v>316</v>
       </c>
       <c r="C961" s="29">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D961" s="29" t="s">
-        <v>1509</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.45">
@@ -27094,10 +27107,10 @@
         <v>316</v>
       </c>
       <c r="C962" s="29">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D962" s="29" t="s">
-        <v>1510</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.45">
@@ -27108,10 +27121,10 @@
         <v>316</v>
       </c>
       <c r="C963" s="29">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D963" s="29" t="s">
-        <v>1511</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.45">
@@ -27122,10 +27135,10 @@
         <v>316</v>
       </c>
       <c r="C964" s="29">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D964" s="29" t="s">
-        <v>1512</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.45">
@@ -27136,10 +27149,10 @@
         <v>316</v>
       </c>
       <c r="C965" s="29">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D965" s="29" t="s">
-        <v>1492</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.45">
@@ -27150,10 +27163,10 @@
         <v>316</v>
       </c>
       <c r="C966" s="29">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D966" s="29" t="s">
-        <v>1493</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.45">
@@ -27164,10 +27177,10 @@
         <v>316</v>
       </c>
       <c r="C967" s="29">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D967" s="29" t="s">
-        <v>1494</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.45">
@@ -27178,10 +27191,10 @@
         <v>316</v>
       </c>
       <c r="C968" s="29">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D968" s="29" t="s">
-        <v>1487</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.45">
@@ -27192,10 +27205,10 @@
         <v>316</v>
       </c>
       <c r="C969" s="29">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D969" s="29" t="s">
-        <v>1468</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.45">
@@ -27206,12 +27219,11 @@
         <v>316</v>
       </c>
       <c r="C970" s="29">
-        <v>901</v>
+        <v>134</v>
       </c>
       <c r="D970" s="29" t="s">
-        <v>1536</v>
-      </c>
-      <c r="E970" s="3"/>
+        <v>1494</v>
+      </c>
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A971" s="29">
@@ -27221,12 +27233,11 @@
         <v>316</v>
       </c>
       <c r="C971" s="29">
-        <v>902</v>
-      </c>
-      <c r="D971" s="28" t="s">
-        <v>1537</v>
-      </c>
-      <c r="E971" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="D971" s="29" t="s">
+        <v>1487</v>
+      </c>
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A972" s="29">
@@ -27236,12 +27247,11 @@
         <v>316</v>
       </c>
       <c r="C972" s="29">
-        <v>903</v>
-      </c>
-      <c r="D972" s="28" t="s">
-        <v>1538</v>
-      </c>
-      <c r="E972" s="3"/>
+        <v>136</v>
+      </c>
+      <c r="D972" s="29" t="s">
+        <v>1468</v>
+      </c>
     </row>
     <row r="973" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A973" s="29">
@@ -27251,10 +27261,10 @@
         <v>316</v>
       </c>
       <c r="C973" s="29">
-        <v>904</v>
-      </c>
-      <c r="D973" s="28" t="s">
-        <v>1539</v>
+        <v>901</v>
+      </c>
+      <c r="D973" s="29" t="s">
+        <v>1536</v>
       </c>
       <c r="E973" s="3"/>
     </row>
@@ -27266,10 +27276,10 @@
         <v>316</v>
       </c>
       <c r="C974" s="29">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="D974" s="28" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
       <c r="E974" s="3"/>
     </row>
@@ -27281,10 +27291,10 @@
         <v>316</v>
       </c>
       <c r="C975" s="29">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="D975" s="28" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
       <c r="E975" s="3"/>
     </row>
@@ -27296,10 +27306,10 @@
         <v>316</v>
       </c>
       <c r="C976" s="29">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="D976" s="28" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="E976" s="3"/>
     </row>
@@ -27311,10 +27321,10 @@
         <v>316</v>
       </c>
       <c r="C977" s="29">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D977" s="28" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="E977" s="3"/>
     </row>
@@ -27326,10 +27336,10 @@
         <v>316</v>
       </c>
       <c r="C978" s="29">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="D978" s="28" t="s">
-        <v>1544</v>
+        <v>1541</v>
       </c>
       <c r="E978" s="3"/>
     </row>
@@ -27341,10 +27351,10 @@
         <v>316</v>
       </c>
       <c r="C979" s="29">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="D979" s="28" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="E979" s="3"/>
     </row>
@@ -27356,10 +27366,10 @@
         <v>316</v>
       </c>
       <c r="C980" s="29">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="D980" s="28" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
       <c r="E980" s="3"/>
     </row>
@@ -27371,10 +27381,10 @@
         <v>316</v>
       </c>
       <c r="C981" s="29">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D981" s="28" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="E981" s="3"/>
     </row>
@@ -27386,10 +27396,10 @@
         <v>316</v>
       </c>
       <c r="C982" s="29">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D982" s="28" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
       <c r="E982" s="3"/>
     </row>
@@ -27401,10 +27411,10 @@
         <v>316</v>
       </c>
       <c r="C983" s="29">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="D983" s="28" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
       <c r="E983" s="3"/>
     </row>
@@ -27416,10 +27426,10 @@
         <v>316</v>
       </c>
       <c r="C984" s="29">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="D984" s="28" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
       <c r="E984" s="3"/>
     </row>
@@ -27431,10 +27441,10 @@
         <v>316</v>
       </c>
       <c r="C985" s="29">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="D985" s="28" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="E985" s="3"/>
     </row>
@@ -27446,10 +27456,10 @@
         <v>316</v>
       </c>
       <c r="C986" s="29">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="D986" s="28" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
       <c r="E986" s="3"/>
     </row>
@@ -27461,10 +27471,10 @@
         <v>316</v>
       </c>
       <c r="C987" s="29">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="D987" s="28" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="E987" s="3"/>
     </row>
@@ -27476,10 +27486,10 @@
         <v>316</v>
       </c>
       <c r="C988" s="29">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="D988" s="28" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
       <c r="E988" s="3"/>
     </row>
@@ -27491,81 +27501,84 @@
         <v>316</v>
       </c>
       <c r="C989" s="29">
-        <v>920</v>
-      </c>
-      <c r="D989" s="29" t="s">
-        <v>1555</v>
+        <v>917</v>
+      </c>
+      <c r="D989" s="28" t="s">
+        <v>1552</v>
       </c>
       <c r="E989" s="3"/>
     </row>
     <row r="990" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A990" s="29">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B990" s="29" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="C990" s="29">
-        <v>0</v>
-      </c>
-      <c r="D990" s="29" t="s">
-        <v>1102</v>
-      </c>
+        <v>918</v>
+      </c>
+      <c r="D990" s="28" t="s">
+        <v>1553</v>
+      </c>
+      <c r="E990" s="3"/>
     </row>
     <row r="991" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A991" s="29">
+        <v>33</v>
+      </c>
+      <c r="B991" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="C991" s="29">
+        <v>919</v>
+      </c>
+      <c r="D991" s="28" t="s">
+        <v>1554</v>
+      </c>
+      <c r="E991" s="3"/>
+    </row>
+    <row r="992" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A992" s="29">
+        <v>33</v>
+      </c>
+      <c r="B992" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="C992" s="29">
+        <v>920</v>
+      </c>
+      <c r="D992" s="29" t="s">
+        <v>1555</v>
+      </c>
+      <c r="E992" s="3"/>
+    </row>
+    <row r="993" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A993" s="29">
         <v>34</v>
       </c>
-      <c r="B991" s="29" t="s">
+      <c r="B993" s="29" t="s">
         <v>330</v>
       </c>
-      <c r="C991" s="29">
+      <c r="C993" s="29">
+        <v>0</v>
+      </c>
+      <c r="D993" s="29" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="994" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A994" s="29">
+        <v>34</v>
+      </c>
+      <c r="B994" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="C994" s="29">
         <v>1</v>
       </c>
-      <c r="D991" s="29" t="s">
+      <c r="D994" s="29" t="s">
         <v>1103</v>
-      </c>
-    </row>
-    <row r="992" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A992">
-        <v>34</v>
-      </c>
-      <c r="B992" t="s">
-        <v>330</v>
-      </c>
-      <c r="C992">
-        <v>2</v>
-      </c>
-      <c r="D992" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="993" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A993">
-        <v>34</v>
-      </c>
-      <c r="B993" t="s">
-        <v>330</v>
-      </c>
-      <c r="C993">
-        <v>3</v>
-      </c>
-      <c r="D993" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="994" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A994">
-        <v>34</v>
-      </c>
-      <c r="B994" t="s">
-        <v>330</v>
-      </c>
-      <c r="C994">
-        <v>8</v>
-      </c>
-      <c r="D994" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="995" spans="1:4" x14ac:dyDescent="0.45">
@@ -27576,10 +27589,10 @@
         <v>330</v>
       </c>
       <c r="C995">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D995" t="s">
-        <v>677</v>
+        <v>636</v>
       </c>
     </row>
     <row r="996" spans="1:4" x14ac:dyDescent="0.45">
@@ -27590,10 +27603,10 @@
         <v>330</v>
       </c>
       <c r="C996">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D996" t="s">
-        <v>678</v>
+        <v>571</v>
       </c>
     </row>
     <row r="997" spans="1:4" x14ac:dyDescent="0.45">
@@ -27604,164 +27617,164 @@
         <v>330</v>
       </c>
       <c r="C997">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D997" t="s">
-        <v>679</v>
+        <v>637</v>
       </c>
     </row>
     <row r="998" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A998" s="29">
-        <v>35</v>
-      </c>
-      <c r="B998" s="29" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C998" s="29">
-        <v>1</v>
-      </c>
-      <c r="D998" s="29" t="s">
-        <v>1105</v>
+      <c r="A998">
+        <v>34</v>
+      </c>
+      <c r="B998" t="s">
+        <v>330</v>
+      </c>
+      <c r="C998">
+        <v>9</v>
+      </c>
+      <c r="D998" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="999" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A999" s="29">
-        <v>35</v>
-      </c>
-      <c r="B999" s="29" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C999" s="29">
-        <v>2</v>
-      </c>
-      <c r="D999" s="29" t="s">
-        <v>1106</v>
+      <c r="A999">
+        <v>34</v>
+      </c>
+      <c r="B999" t="s">
+        <v>330</v>
+      </c>
+      <c r="C999">
+        <v>10</v>
+      </c>
+      <c r="D999" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="1000" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1000">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1000" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C1000">
+        <v>13</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1001" s="29">
+        <v>35</v>
+      </c>
+      <c r="B1001" s="29" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C1001" s="29">
         <v>1</v>
       </c>
-      <c r="D1000" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="1001" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1001">
-        <v>36</v>
-      </c>
-      <c r="B1001" t="s">
-        <v>333</v>
-      </c>
-      <c r="C1001">
-        <v>3</v>
-      </c>
-      <c r="D1001" t="s">
-        <v>511</v>
+      <c r="D1001" s="29" t="s">
+        <v>1105</v>
       </c>
     </row>
     <row r="1002" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1002">
-        <v>36</v>
-      </c>
-      <c r="B1002" t="s">
-        <v>333</v>
-      </c>
-      <c r="C1002">
-        <v>4</v>
-      </c>
-      <c r="D1002" t="s">
-        <v>512</v>
+      <c r="A1002" s="29">
+        <v>35</v>
+      </c>
+      <c r="B1002" s="29" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C1002" s="29">
+        <v>2</v>
+      </c>
+      <c r="D1002" s="29" t="s">
+        <v>1106</v>
       </c>
     </row>
     <row r="1003" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1003">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1003" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C1003">
         <v>1</v>
       </c>
       <c r="D1003" t="s">
-        <v>479</v>
+        <v>510</v>
       </c>
     </row>
     <row r="1004" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1004">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1004" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C1004">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1004" t="s">
-        <v>480</v>
+        <v>511</v>
       </c>
     </row>
     <row r="1005" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1005">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1005" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C1005">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1005" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
     </row>
     <row r="1006" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1006">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1006" t="s">
-        <v>20</v>
+        <v>331</v>
       </c>
       <c r="C1006">
         <v>1</v>
       </c>
       <c r="D1006" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="1007" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1007">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1007" t="s">
-        <v>20</v>
+        <v>331</v>
       </c>
       <c r="C1007">
         <v>2</v>
       </c>
       <c r="D1007" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="1008" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1008">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1008" t="s">
-        <v>20</v>
+        <v>331</v>
       </c>
       <c r="C1008">
         <v>3</v>
       </c>
       <c r="D1008" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="1009" spans="1:4" x14ac:dyDescent="0.45">
@@ -27772,10 +27785,10 @@
         <v>20</v>
       </c>
       <c r="C1009">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1009" t="s">
-        <v>680</v>
+        <v>482</v>
       </c>
     </row>
     <row r="1010" spans="1:4" x14ac:dyDescent="0.45">
@@ -27786,10 +27799,10 @@
         <v>20</v>
       </c>
       <c r="C1010">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1010" t="s">
-        <v>681</v>
+        <v>483</v>
       </c>
     </row>
     <row r="1011" spans="1:4" x14ac:dyDescent="0.45">
@@ -27800,10 +27813,10 @@
         <v>20</v>
       </c>
       <c r="C1011">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1011" t="s">
-        <v>682</v>
+        <v>484</v>
       </c>
     </row>
     <row r="1012" spans="1:4" x14ac:dyDescent="0.45">
@@ -27814,10 +27827,10 @@
         <v>20</v>
       </c>
       <c r="C1012">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1012" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="1013" spans="1:4" x14ac:dyDescent="0.45">
@@ -27828,10 +27841,10 @@
         <v>20</v>
       </c>
       <c r="C1013">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1013" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="1014" spans="1:4" x14ac:dyDescent="0.45">
@@ -27842,10 +27855,10 @@
         <v>20</v>
       </c>
       <c r="C1014">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1014" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="1015" spans="1:4" x14ac:dyDescent="0.45">
@@ -27856,10 +27869,10 @@
         <v>20</v>
       </c>
       <c r="C1015">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1015" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="1016" spans="1:4" x14ac:dyDescent="0.45">
@@ -27870,10 +27883,10 @@
         <v>20</v>
       </c>
       <c r="C1016">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1016" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="1017" spans="1:4" x14ac:dyDescent="0.45">
@@ -27884,10 +27897,10 @@
         <v>20</v>
       </c>
       <c r="C1017">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1017" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="1018" spans="1:4" x14ac:dyDescent="0.45">
@@ -27898,10 +27911,10 @@
         <v>20</v>
       </c>
       <c r="C1018">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1018" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="1019" spans="1:4" x14ac:dyDescent="0.45">
@@ -27912,10 +27925,10 @@
         <v>20</v>
       </c>
       <c r="C1019">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1019" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="1020" spans="1:4" x14ac:dyDescent="0.45">
@@ -27926,10 +27939,10 @@
         <v>20</v>
       </c>
       <c r="C1020">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D1020" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="1021" spans="1:4" x14ac:dyDescent="0.45">
@@ -27940,10 +27953,10 @@
         <v>20</v>
       </c>
       <c r="C1021">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D1021" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="1022" spans="1:4" x14ac:dyDescent="0.45">
@@ -27954,10 +27967,10 @@
         <v>20</v>
       </c>
       <c r="C1022">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D1022" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="1023" spans="1:4" x14ac:dyDescent="0.45">
@@ -27968,10 +27981,10 @@
         <v>20</v>
       </c>
       <c r="C1023">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D1023" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="1024" spans="1:4" x14ac:dyDescent="0.45">
@@ -27982,10 +27995,10 @@
         <v>20</v>
       </c>
       <c r="C1024">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1024" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="1025" spans="1:4" x14ac:dyDescent="0.45">
@@ -27996,10 +28009,10 @@
         <v>20</v>
       </c>
       <c r="C1025">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1025" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="1026" spans="1:4" x14ac:dyDescent="0.45">
@@ -28010,10 +28023,10 @@
         <v>20</v>
       </c>
       <c r="C1026">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D1026" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="1027" spans="1:4" x14ac:dyDescent="0.45">
@@ -28024,10 +28037,10 @@
         <v>20</v>
       </c>
       <c r="C1027">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1027" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="1028" spans="1:4" x14ac:dyDescent="0.45">
@@ -28038,10 +28051,10 @@
         <v>20</v>
       </c>
       <c r="C1028">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1028" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="1029" spans="1:4" x14ac:dyDescent="0.45">
@@ -28052,10 +28065,10 @@
         <v>20</v>
       </c>
       <c r="C1029">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1029" t="s">
-        <v>485</v>
+        <v>697</v>
       </c>
     </row>
     <row r="1030" spans="1:4" x14ac:dyDescent="0.45">
@@ -28066,10 +28079,10 @@
         <v>20</v>
       </c>
       <c r="C1030">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1030" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="1031" spans="1:4" x14ac:dyDescent="0.45">
@@ -28080,10 +28093,10 @@
         <v>20</v>
       </c>
       <c r="C1031">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D1031" t="s">
-        <v>486</v>
+        <v>699</v>
       </c>
     </row>
     <row r="1032" spans="1:4" x14ac:dyDescent="0.45">
@@ -28094,10 +28107,10 @@
         <v>20</v>
       </c>
       <c r="C1032">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D1032" t="s">
-        <v>701</v>
+        <v>485</v>
       </c>
     </row>
     <row r="1033" spans="1:4" x14ac:dyDescent="0.45">
@@ -28108,10 +28121,10 @@
         <v>20</v>
       </c>
       <c r="C1033">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D1033" t="s">
-        <v>487</v>
+        <v>700</v>
       </c>
     </row>
     <row r="1034" spans="1:4" x14ac:dyDescent="0.45">
@@ -28122,10 +28135,10 @@
         <v>20</v>
       </c>
       <c r="C1034">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D1034" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="1035" spans="1:4" x14ac:dyDescent="0.45">
@@ -28136,10 +28149,10 @@
         <v>20</v>
       </c>
       <c r="C1035">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D1035" t="s">
-        <v>512</v>
+        <v>701</v>
       </c>
     </row>
     <row r="1036" spans="1:4" x14ac:dyDescent="0.45">
@@ -28150,10 +28163,10 @@
         <v>20</v>
       </c>
       <c r="C1036">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D1036" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="1037" spans="1:4" x14ac:dyDescent="0.45">
@@ -28164,10 +28177,10 @@
         <v>20</v>
       </c>
       <c r="C1037">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D1037" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="1038" spans="1:4" x14ac:dyDescent="0.45">
@@ -28178,10 +28191,10 @@
         <v>20</v>
       </c>
       <c r="C1038">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D1038" t="s">
-        <v>491</v>
+        <v>512</v>
       </c>
     </row>
     <row r="1039" spans="1:4" x14ac:dyDescent="0.45">
@@ -28192,10 +28205,10 @@
         <v>20</v>
       </c>
       <c r="C1039">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D1039" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="1040" spans="1:4" x14ac:dyDescent="0.45">
@@ -28206,10 +28219,10 @@
         <v>20</v>
       </c>
       <c r="C1040">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D1040" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="1041" spans="1:4" x14ac:dyDescent="0.45">
@@ -28220,10 +28233,10 @@
         <v>20</v>
       </c>
       <c r="C1041">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1041" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="1042" spans="1:4" x14ac:dyDescent="0.45">
@@ -28234,10 +28247,10 @@
         <v>20</v>
       </c>
       <c r="C1042">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D1042" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="1043" spans="1:4" x14ac:dyDescent="0.45">
@@ -28248,10 +28261,10 @@
         <v>20</v>
       </c>
       <c r="C1043">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1043" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="1044" spans="1:4" x14ac:dyDescent="0.45">
@@ -28262,10 +28275,10 @@
         <v>20</v>
       </c>
       <c r="C1044">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D1044" t="s">
-        <v>702</v>
+        <v>494</v>
       </c>
     </row>
     <row r="1045" spans="1:4" x14ac:dyDescent="0.45">
@@ -28276,10 +28289,10 @@
         <v>20</v>
       </c>
       <c r="C1045">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1045" t="s">
-        <v>703</v>
+        <v>495</v>
       </c>
     </row>
     <row r="1046" spans="1:4" x14ac:dyDescent="0.45">
@@ -28290,10 +28303,10 @@
         <v>20</v>
       </c>
       <c r="C1046">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1046" t="s">
-        <v>704</v>
+        <v>496</v>
       </c>
     </row>
     <row r="1047" spans="1:4" x14ac:dyDescent="0.45">
@@ -28304,10 +28317,10 @@
         <v>20</v>
       </c>
       <c r="C1047">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1047" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="1048" spans="1:4" x14ac:dyDescent="0.45">
@@ -28318,10 +28331,10 @@
         <v>20</v>
       </c>
       <c r="C1048">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1048" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="1049" spans="1:4" x14ac:dyDescent="0.45">
@@ -28332,10 +28345,10 @@
         <v>20</v>
       </c>
       <c r="C1049">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1049" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="1050" spans="1:4" x14ac:dyDescent="0.45">
@@ -28346,10 +28359,10 @@
         <v>20</v>
       </c>
       <c r="C1050">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D1050" t="s">
-        <v>497</v>
+        <v>705</v>
       </c>
     </row>
     <row r="1051" spans="1:4" x14ac:dyDescent="0.45">
@@ -28360,10 +28373,10 @@
         <v>20</v>
       </c>
       <c r="C1051">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1051" t="s">
-        <v>498</v>
+        <v>706</v>
       </c>
     </row>
     <row r="1052" spans="1:4" x14ac:dyDescent="0.45">
@@ -28374,10 +28387,10 @@
         <v>20</v>
       </c>
       <c r="C1052">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D1052" t="s">
-        <v>499</v>
+        <v>707</v>
       </c>
     </row>
     <row r="1053" spans="1:4" x14ac:dyDescent="0.45">
@@ -28387,11 +28400,11 @@
       <c r="B1053" t="s">
         <v>20</v>
       </c>
-      <c r="C1053" s="29">
-        <v>53</v>
-      </c>
-      <c r="D1053" s="29" t="s">
-        <v>1519</v>
+      <c r="C1053">
+        <v>50</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="1054" spans="1:4" x14ac:dyDescent="0.45">
@@ -28401,11 +28414,11 @@
       <c r="B1054" t="s">
         <v>20</v>
       </c>
-      <c r="C1054" s="29">
-        <v>54</v>
-      </c>
-      <c r="D1054" s="29" t="s">
-        <v>1518</v>
+      <c r="C1054">
+        <v>51</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="1055" spans="1:4" x14ac:dyDescent="0.45">
@@ -28415,179 +28428,179 @@
       <c r="B1055" t="s">
         <v>20</v>
       </c>
-      <c r="C1055" s="29">
-        <v>55</v>
-      </c>
-      <c r="D1055" s="29" t="s">
-        <v>1517</v>
+      <c r="C1055">
+        <v>52</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="1056" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1056">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1056" t="s">
-        <v>500</v>
-      </c>
-      <c r="C1056">
-        <v>1</v>
-      </c>
-      <c r="D1056" t="s">
-        <v>501</v>
+        <v>20</v>
+      </c>
+      <c r="C1056" s="29">
+        <v>53</v>
+      </c>
+      <c r="D1056" s="29" t="s">
+        <v>1519</v>
       </c>
     </row>
     <row r="1057" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1057">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1057" t="s">
-        <v>500</v>
-      </c>
-      <c r="C1057">
-        <v>3</v>
-      </c>
-      <c r="D1057" t="s">
-        <v>502</v>
+        <v>20</v>
+      </c>
+      <c r="C1057" s="29">
+        <v>54</v>
+      </c>
+      <c r="D1057" s="29" t="s">
+        <v>1518</v>
       </c>
     </row>
     <row r="1058" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1058">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1058" t="s">
-        <v>500</v>
-      </c>
-      <c r="C1058">
-        <v>4</v>
-      </c>
-      <c r="D1058" t="s">
-        <v>503</v>
+        <v>20</v>
+      </c>
+      <c r="C1058" s="29">
+        <v>55</v>
+      </c>
+      <c r="D1058" s="29" t="s">
+        <v>1517</v>
       </c>
     </row>
     <row r="1059" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1059">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1059" t="s">
-        <v>351</v>
+        <v>500</v>
       </c>
       <c r="C1059">
         <v>1</v>
       </c>
       <c r="D1059" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="1060" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1060">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1060" t="s">
-        <v>351</v>
+        <v>500</v>
       </c>
       <c r="C1060">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1060" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="1061" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1061">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1061" t="s">
-        <v>351</v>
+        <v>500</v>
       </c>
       <c r="C1061">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1061" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
     </row>
     <row r="1062" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1062">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1062" t="s">
-        <v>504</v>
+        <v>351</v>
       </c>
       <c r="C1062">
         <v>1</v>
       </c>
       <c r="D1062" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="1063" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1063">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1063" t="s">
-        <v>504</v>
+        <v>351</v>
       </c>
       <c r="C1063">
         <v>2</v>
       </c>
       <c r="D1063" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="1064" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1064">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1064" t="s">
-        <v>504</v>
+        <v>351</v>
       </c>
       <c r="C1064">
         <v>3</v>
       </c>
       <c r="D1064" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
     </row>
     <row r="1065" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1065">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1065" t="s">
-        <v>348</v>
+        <v>504</v>
       </c>
       <c r="C1065">
         <v>1</v>
       </c>
       <c r="D1065" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
     </row>
     <row r="1066" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1066">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1066" t="s">
-        <v>348</v>
+        <v>504</v>
       </c>
       <c r="C1066">
         <v>2</v>
       </c>
       <c r="D1066" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
     </row>
     <row r="1067" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1067">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1067" t="s">
-        <v>348</v>
+        <v>504</v>
       </c>
       <c r="C1067">
         <v>3</v>
       </c>
       <c r="D1067" t="s">
-        <v>516</v>
+        <v>478</v>
       </c>
     </row>
     <row r="1068" spans="1:4" x14ac:dyDescent="0.45">
@@ -28598,52 +28611,52 @@
         <v>348</v>
       </c>
       <c r="C1068">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="D1068" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="1069" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1069">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1069" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1069" s="29">
-        <v>0</v>
-      </c>
-      <c r="D1069" s="29" t="s">
-        <v>1522</v>
+        <v>348</v>
+      </c>
+      <c r="C1069">
+        <v>2</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="1070" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1070">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1070" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1070" s="29">
-        <v>1</v>
-      </c>
-      <c r="D1070" s="29" t="s">
-        <v>708</v>
+        <v>348</v>
+      </c>
+      <c r="C1070">
+        <v>3</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="1071" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1071">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1071" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1071" s="29">
-        <v>2</v>
-      </c>
-      <c r="D1071" s="29" t="s">
-        <v>711</v>
+        <v>348</v>
+      </c>
+      <c r="C1071">
+        <v>99</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="1072" spans="1:4" x14ac:dyDescent="0.45">
@@ -28654,10 +28667,10 @@
         <v>75</v>
       </c>
       <c r="C1072" s="29">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1072" s="29" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1073" spans="1:4" x14ac:dyDescent="0.45">
@@ -28668,10 +28681,10 @@
         <v>75</v>
       </c>
       <c r="C1073" s="29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1073" s="29" t="s">
-        <v>1524</v>
+        <v>708</v>
       </c>
     </row>
     <row r="1074" spans="1:4" x14ac:dyDescent="0.45">
@@ -28682,60 +28695,60 @@
         <v>75</v>
       </c>
       <c r="C1074" s="29">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1074" s="29" t="s">
-        <v>1525</v>
+        <v>711</v>
       </c>
     </row>
     <row r="1075" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1075">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1075" t="s">
-        <v>758</v>
-      </c>
-      <c r="C1075">
-        <v>0</v>
-      </c>
-      <c r="D1075" t="s">
-        <v>476</v>
+        <v>75</v>
+      </c>
+      <c r="C1075" s="29">
+        <v>3</v>
+      </c>
+      <c r="D1075" s="29" t="s">
+        <v>1523</v>
       </c>
     </row>
     <row r="1076" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1076">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1076" t="s">
-        <v>758</v>
-      </c>
-      <c r="C1076">
-        <v>1</v>
-      </c>
-      <c r="D1076" t="s">
-        <v>477</v>
+        <v>75</v>
+      </c>
+      <c r="C1076" s="29">
+        <v>4</v>
+      </c>
+      <c r="D1076" s="29" t="s">
+        <v>1524</v>
       </c>
     </row>
     <row r="1077" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1077">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1077" t="s">
-        <v>758</v>
-      </c>
-      <c r="C1077">
-        <v>-1</v>
-      </c>
-      <c r="D1077" t="s">
-        <v>512</v>
+        <v>75</v>
+      </c>
+      <c r="C1077" s="29">
+        <v>9</v>
+      </c>
+      <c r="D1077" s="29" t="s">
+        <v>1525</v>
       </c>
     </row>
     <row r="1078" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1078">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1078" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C1078">
         <v>0</v>
@@ -28746,10 +28759,10 @@
     </row>
     <row r="1079" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1079">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1079" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C1079">
         <v>1</v>
@@ -28760,58 +28773,58 @@
     </row>
     <row r="1080" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1080">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1080" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C1080">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D1080" t="s">
-        <v>760</v>
+        <v>512</v>
       </c>
     </row>
     <row r="1081" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1081">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1081" t="s">
-        <v>199</v>
+        <v>759</v>
       </c>
       <c r="C1081">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D1081" t="s">
-        <v>512</v>
+        <v>476</v>
       </c>
     </row>
     <row r="1082" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1082">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1082" t="s">
-        <v>199</v>
+        <v>759</v>
       </c>
       <c r="C1082">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1082" t="s">
-        <v>763</v>
+        <v>477</v>
       </c>
     </row>
     <row r="1083" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1083">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1083" t="s">
-        <v>199</v>
+        <v>759</v>
       </c>
       <c r="C1083">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1083" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
     </row>
     <row r="1084" spans="1:4" x14ac:dyDescent="0.45">
@@ -28822,98 +28835,140 @@
         <v>199</v>
       </c>
       <c r="C1084">
+        <v>-1</v>
+      </c>
+      <c r="D1084" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1085">
+        <v>46</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1085">
+        <v>0</v>
+      </c>
+      <c r="D1085" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1086">
+        <v>46</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1086">
+        <v>1</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1087">
+        <v>46</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1087">
         <v>99</v>
       </c>
-      <c r="D1084" t="s">
+      <c r="D1087" t="s">
         <v>569</v>
-      </c>
-    </row>
-    <row r="1085" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1085" s="29">
-        <v>47</v>
-      </c>
-      <c r="B1085" s="29" t="s">
-        <v>1128</v>
-      </c>
-      <c r="C1085" s="29">
-        <v>0</v>
-      </c>
-      <c r="D1085" s="29" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="1086" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1086" s="29">
-        <v>47</v>
-      </c>
-      <c r="B1086" s="29" t="s">
-        <v>1128</v>
-      </c>
-      <c r="C1086" s="29">
-        <v>1</v>
-      </c>
-      <c r="D1086" s="29" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="1087" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1087" s="29">
-        <v>47</v>
-      </c>
-      <c r="B1087" s="29" t="s">
-        <v>1128</v>
-      </c>
-      <c r="C1087" s="29">
-        <v>2</v>
-      </c>
-      <c r="D1087" s="29" t="s">
-        <v>1133</v>
       </c>
     </row>
     <row r="1088" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1088" s="29">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1088" s="29" t="s">
-        <v>80</v>
+        <v>1128</v>
       </c>
       <c r="C1088" s="29">
         <v>0</v>
       </c>
       <c r="D1088" s="29" t="s">
-        <v>1520</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1089" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1089" s="29">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1089" s="29" t="s">
-        <v>80</v>
+        <v>1128</v>
       </c>
       <c r="C1089" s="29">
         <v>1</v>
       </c>
       <c r="D1089" s="29" t="s">
-        <v>410</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1090" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1090" s="29">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1090" s="29" t="s">
-        <v>80</v>
+        <v>1128</v>
       </c>
       <c r="C1090" s="29">
         <v>2</v>
       </c>
       <c r="D1090" s="29" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1091" s="29">
+        <v>48</v>
+      </c>
+      <c r="B1091" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1091" s="29">
+        <v>0</v>
+      </c>
+      <c r="D1091" s="29" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1092" s="29">
+        <v>48</v>
+      </c>
+      <c r="B1092" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1092" s="29">
+        <v>1</v>
+      </c>
+      <c r="D1092" s="29" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1093" s="29">
+        <v>48</v>
+      </c>
+      <c r="B1093" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1093" s="29">
+        <v>2</v>
+      </c>
+      <c r="D1093" s="29" t="s">
         <v>1521</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XFB1090" xr:uid="{5B52880F-20AD-49BC-9FD8-A02C6FD116A7}"/>
+  <autoFilter ref="A1:XFB1093" xr:uid="{5B52880F-20AD-49BC-9FD8-A02C6FD116A7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C219:D257">
     <sortCondition ref="C219:C257"/>
   </sortState>

</xml_diff>